<commit_message>
Add spamassassin setup codes
</commit_message>
<xml_diff>
--- a/project/spam_mail_detection/연람희_주간&일일보고_210911.xlsx
+++ b/project/spam_mail_detection/연람희_주간&일일보고_210911.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramie\OneDrive\Documents\learn_programming\project\spam_mail_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B202E9-AB6B-4110-84E1-1662F49F0E8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD9F567-EEE5-48CB-A7BD-C40BA32FFEF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{03C89AB5-3466-4C93-B69B-4E1CD49D46A7}"/>
   </bookViews>
@@ -103,7 +103,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> - DNS 서부 구축, 메일 수신 확인</t>
+    <t xml:space="preserve"> - Spamassassin sendmail 연동. Spamassassin에 딥러닝을 어떻게 연결할 수 있는지 분석</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E7B2D1-3763-4111-936D-623F04C23C6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -610,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2">
-        <v>44450</v>
+        <v>44451</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Update procmailrc running through Py script
</commit_message>
<xml_diff>
--- a/project/spam_mail_detection/연람희_주간&일일보고_210911.xlsx
+++ b/project/spam_mail_detection/연람희_주간&일일보고_210911.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramie\OneDrive\Documents\learn_programming\project\spam_mail_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B06715-5899-46FF-8435-94E7498DE4B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAE0FC3-BF6B-4852-8CB6-25769DFD0718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{03C89AB5-3466-4C93-B69B-4E1CD49D46A7}"/>
   </bookViews>
@@ -101,7 +101,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> - SA local rule로 파이썬 스크립트를 구동 가능하도록 적용
+    <t xml:space="preserve"> - SA 를 파이썬 스크립트를 구동 가능하도록 적용
  - 외부에서 VM으로 메일이 올 수 있도록 port forwarding 공부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E7B2D1-3763-4111-936D-623F04C23C6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Add with open claus in python code
</commit_message>
<xml_diff>
--- a/project/spam_mail_detection/연람희_주간&일일보고_210911.xlsx
+++ b/project/spam_mail_detection/연람희_주간&일일보고_210911.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramie\OneDrive\Documents\learn_programming\project\spam_mail_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAE0FC3-BF6B-4852-8CB6-25769DFD0718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4989B9F-5B49-454E-9803-E2AD9FD7F02F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{03C89AB5-3466-4C93-B69B-4E1CD49D46A7}"/>
   </bookViews>
@@ -83,10 +83,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> - SA을 파이썬 스크립트로 스팸 점수를 부여할 수 있는지 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>지난주 업무
 (09.17 - 09.24)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +99,10 @@
   <si>
     <t xml:space="preserve"> - SA 를 파이썬 스크립트를 구동 가능하도록 적용
  - 외부에서 VM으로 메일이 올 수 있도록 port forwarding 공부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>procmailrc-&gt;python script 연결</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E7B2D1-3763-4111-936D-623F04C23C6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -661,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="5"/>
@@ -691,10 +691,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>13</v>
@@ -721,10 +721,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="D19" s="5"/>
     </row>

</xml_diff>